<commit_message>
added local volume for code changes, updated tests
</commit_message>
<xml_diff>
--- a/metro2/tests/test.xlsx
+++ b/metro2/tests/test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seiferc/Documents/Metro2/metro2/tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seiferc/Documents/internal-products/metro2/metro2/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1504586-43ED-DC40-8B71-6E4A9BF7CDD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0356C9C5-80A6-5C43-B1AC-DAC25631925D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15760" activeTab="1" xr2:uid="{C849C475-6124-2A43-A001-3349402AD2D1}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
   <si>
     <t>segment</t>
   </si>
@@ -52,6 +52,36 @@
   </si>
   <si>
     <t>base</t>
+  </si>
+  <si>
+    <t>field1</t>
+  </si>
+  <si>
+    <t>field2</t>
+  </si>
+  <si>
+    <t>field3</t>
+  </si>
+  <si>
+    <t>field4</t>
+  </si>
+  <si>
+    <t>field5</t>
+  </si>
+  <si>
+    <t>field1_base</t>
+  </si>
+  <si>
+    <t>field2_base</t>
+  </si>
+  <si>
+    <t>field3_base</t>
+  </si>
+  <si>
+    <t>field4_base</t>
+  </si>
+  <si>
+    <t>field5_base</t>
   </si>
 </sst>
 </file>
@@ -415,15 +445,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ECCE883-75CE-E849-BD26-BC588344B998}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -434,7 +464,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -444,8 +474,11 @@
       <c r="C2">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -455,8 +488,11 @@
       <c r="C3">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -466,8 +502,11 @@
       <c r="C4">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -477,8 +516,11 @@
       <c r="C5">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -488,8 +530,11 @@
       <c r="C6">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -499,8 +544,11 @@
       <c r="C7">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -510,8 +558,11 @@
       <c r="C8">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -521,8 +572,11 @@
       <c r="C9">
         <v>24</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -532,8 +586,11 @@
       <c r="C10">
         <v>26</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -542,6 +599,9 @@
       </c>
       <c r="C11">
         <v>100</v>
+      </c>
+      <c r="D11" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>